<commit_message>
some stuff for restructure, new fighters, ...
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{979206C8-114A-4269-A9CB-43A52319E3D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7F425A-B1CE-4244-8962-D37621750C9B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="301">
   <si>
     <t>Guard</t>
   </si>
@@ -665,13 +665,286 @@
   </si>
   <si>
     <t>Cinder</t>
+  </si>
+  <si>
+    <t>Bronze:</t>
+  </si>
+  <si>
+    <t>Image By:</t>
+  </si>
+  <si>
+    <t>Wood Spectre + 2x Wood Walker</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>Venus Djinn</t>
+  </si>
+  <si>
+    <t>bringobonog</t>
+  </si>
+  <si>
+    <t>Mars Djinn</t>
+  </si>
+  <si>
+    <t>JupiterDjinn</t>
+  </si>
+  <si>
+    <t>Mercury Djinn</t>
+  </si>
+  <si>
+    <t>Antlion</t>
+  </si>
+  <si>
+    <t>Saturos</t>
+  </si>
+  <si>
+    <t>Mimic</t>
+  </si>
+  <si>
+    <t>9x Slimes</t>
+  </si>
+  <si>
+    <t>Wyvern/Gryphon/Wynvern</t>
+  </si>
+  <si>
+    <t>3x Skeleton</t>
+  </si>
+  <si>
+    <t>Sean/Ouranos</t>
+  </si>
+  <si>
+    <t>Azart</t>
+  </si>
+  <si>
+    <t>Thief/Bandit/Thief</t>
+  </si>
+  <si>
+    <t>3x Mauler</t>
+  </si>
+  <si>
+    <t>3x Crab</t>
+  </si>
+  <si>
+    <t>Seafighter</t>
+  </si>
+  <si>
+    <t>Emus</t>
+  </si>
+  <si>
+    <t>Goblins</t>
+  </si>
+  <si>
+    <t>Chestbeaters</t>
+  </si>
+  <si>
+    <t>Moapa Knight</t>
+  </si>
+  <si>
+    <t>King Scorption</t>
+  </si>
+  <si>
+    <t>Mad Plant</t>
+  </si>
+  <si>
+    <t>Tret</t>
+  </si>
+  <si>
+    <t>Feitzhi/Hsu?</t>
+  </si>
+  <si>
+    <t>Kaja</t>
+  </si>
+  <si>
+    <t>Werewolves</t>
+  </si>
+  <si>
+    <t>Dwarfs</t>
+  </si>
+  <si>
+    <t>Living Armor</t>
+  </si>
+  <si>
+    <t>Ghost Army</t>
+  </si>
+  <si>
+    <t>Punch Ants</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Image By</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>TBS Gang</t>
+  </si>
+  <si>
+    <t>TLA Gang</t>
+  </si>
+  <si>
+    <t>Djinn Lineup</t>
+  </si>
+  <si>
+    <t>Piers/Eoleo</t>
+  </si>
+  <si>
+    <t>Hydros Statue + 2x Living Statue</t>
+  </si>
+  <si>
+    <t>Killer Ape + 4x Apes</t>
+  </si>
+  <si>
+    <t>Hobgoblin + 2x Virago</t>
+  </si>
+  <si>
+    <t>Succubus + 2x Grisly</t>
+  </si>
+  <si>
+    <t>Lich + 2x Fiendish Ghoul</t>
+  </si>
+  <si>
+    <t>2x Gryphon</t>
+  </si>
+  <si>
+    <t>Satrage</t>
+  </si>
+  <si>
+    <t>Navampa</t>
+  </si>
+  <si>
+    <t>2x Nue</t>
+  </si>
+  <si>
+    <t>Briggs + 2x seafighter</t>
+  </si>
+  <si>
+    <t>Serpent</t>
+  </si>
+  <si>
+    <t>Minotaurs</t>
+  </si>
+  <si>
+    <t>Susa + Miko + Curse Mage</t>
+  </si>
+  <si>
+    <t>Avimander</t>
+  </si>
+  <si>
+    <t>2x Moapa Knight</t>
+  </si>
+  <si>
+    <t>Menardi</t>
+  </si>
+  <si>
+    <t>Toadonpa</t>
+  </si>
+  <si>
+    <t>Manticore</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image </t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Cursed Saturos</t>
+  </si>
+  <si>
+    <t>Benus Djinn</t>
+  </si>
+  <si>
+    <t>Saturos + Menardi</t>
+  </si>
+  <si>
+    <t>Deadbeard</t>
+  </si>
+  <si>
+    <t>TLA lineup</t>
+  </si>
+  <si>
+    <t>Lizard King</t>
+  </si>
+  <si>
+    <t>2x Chimera</t>
+  </si>
+  <si>
+    <t>2x Earth Lizard</t>
+  </si>
+  <si>
+    <t>Gldiators</t>
+  </si>
+  <si>
+    <t>Poison Toad + 2x Thunder Lizard</t>
+  </si>
+  <si>
+    <t>Succubus + 2x Lich</t>
+  </si>
+  <si>
+    <t>2x Hobgoblin</t>
+  </si>
+  <si>
+    <t>Lizard King + Eath/Thunder</t>
+  </si>
+  <si>
+    <t>Serpent 1</t>
+  </si>
+  <si>
+    <t>Serpent 2</t>
+  </si>
+  <si>
+    <t>Mini Sentinel</t>
+  </si>
+  <si>
+    <t>2x Wonderbird</t>
+  </si>
+  <si>
+    <t>Ogre Titans 1-4</t>
+  </si>
+  <si>
+    <t>Ogre Titan 5</t>
+  </si>
+  <si>
+    <t>Moapa</t>
+  </si>
+  <si>
+    <t>Gabomba</t>
+  </si>
+  <si>
+    <t>Poseidon</t>
+  </si>
+  <si>
+    <t>Mountain Roc</t>
+  </si>
+  <si>
+    <t>Ruffians</t>
+  </si>
+  <si>
+    <t>(Super Slambo)</t>
+  </si>
+  <si>
+    <t>Danny's Fren</t>
+  </si>
+  <si>
+    <t>eLTeh</t>
+  </si>
+  <si>
+    <t>Shuuda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -754,6 +1027,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -808,10 +1087,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -830,9 +1110,16 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{96F5CFF9-578C-433E-B401-E4A3F8FFBEAD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1146,7 +1433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
@@ -2265,4 +2552,397 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F22D4E-FC21-4D0F-B535-11FE6D9F512D}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" style="18" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="18"/>
+    <col min="4" max="4" width="27.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="18"/>
+    <col min="7" max="7" width="15.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="D4" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New Unlocks and Requirements for Page and more
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3079DB-A411-4327-98EF-B9C9E1F3173F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB257B4F-7CF8-4C41-8283-7334F7594E74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4365" windowWidth="21840" windowHeight="13290" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Enemies" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="324">
   <si>
     <t>Guard</t>
   </si>
@@ -682,9 +682,6 @@
     <t>Venus Djinn</t>
   </si>
   <si>
-    <t>bringobonog</t>
-  </si>
-  <si>
     <t>Mars Djinn</t>
   </si>
   <si>
@@ -983,6 +980,33 @@
   </si>
   <si>
     <t>Stealthy Scouts</t>
+  </si>
+  <si>
+    <t>bringobrongo</t>
+  </si>
+  <si>
+    <t>Mono:</t>
+  </si>
+  <si>
+    <t>Dual:</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Unlock</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
+  </si>
+  <si>
+    <t>15 CW</t>
   </si>
 </sst>
 </file>
@@ -1476,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2042,6 +2066,41 @@
       </c>
       <c r="N20" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>316</v>
+      </c>
+      <c r="E25" t="s">
+        <v>319</v>
+      </c>
+      <c r="F25" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" t="s">
+        <v>320</v>
+      </c>
+      <c r="F26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2361,7 +2420,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:J4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2603,8 +2662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F22D4E-FC21-4D0F-B535-11FE6D9F512D}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2625,16 +2684,16 @@
         <v>211</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>246</v>
-      </c>
       <c r="G1" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>270</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2642,59 +2701,59 @@
         <v>214</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>215</v>
+        <v>315</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="19"/>
       <c r="D4" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>213</v>
@@ -2702,27 +2761,27 @@
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>213</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2733,302 +2792,302 @@
         <v>213</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>213</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>213</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various minor changes and fixes
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C0ED3D-E93E-4DAE-A74D-A57518398A7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9D14E-1903-43CD-80D7-C53185F1FCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="2076" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2964,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B53968-0167-4F4F-BD4B-0794225E238B}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2973,7 +2973,7 @@
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3651,8 +3651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC84A19-D4A7-4A92-BABE-05F233968AC8}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Djinn Improvements and Corrections
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9D14E-1903-43CD-80D7-C53185F1FCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D2F6B3-073C-462B-A41E-AF51BCB886AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="2076" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="397">
   <si>
     <t>Guard</t>
   </si>
@@ -984,12 +984,6 @@
     <t>Haunt/Curse/Condemn</t>
   </si>
   <si>
-    <t>Haunt/Curse/ Condemn</t>
-  </si>
-  <si>
-    <t>Sleep/ Delusion</t>
-  </si>
-  <si>
     <t>Curse/Haunt/Weaken/ Delude/Sleep</t>
   </si>
   <si>
@@ -1231,13 +1225,16 @@
   </si>
   <si>
     <t>Morgan</t>
+  </si>
+  <si>
+    <t>Curse/ Condemn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,6 +1264,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1471,7 +1475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1541,6 +1545,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1860,7 +1867,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,23 +2279,23 @@
         <v>314</v>
       </c>
       <c r="B13" s="51" t="s">
+        <v>396</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="C13" s="51" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>316</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>317</v>
-      </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="58" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="51"/>
       <c r="H13" s="51"/>
-      <c r="I13" s="51" t="s">
+      <c r="I13" s="58" t="s">
         <v>80</v>
       </c>
       <c r="J13" s="51" t="s">
@@ -2297,8 +2304,8 @@
       <c r="K13" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="51" t="s">
-        <v>79</v>
+      <c r="L13" s="58" t="s">
+        <v>151</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>312</v>
@@ -2964,7 +2971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B53968-0167-4F4F-BD4B-0794225E238B}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3207,8 +3214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F22D4E-FC21-4D0F-B535-11FE6D9F512D}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="72" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3589,21 +3596,24 @@
       <c r="A28" s="2" t="s">
         <v>218</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>220</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3611,10 +3621,7 @@
         <v>221</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3663,62 +3670,62 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L3" s="55"/>
       <c r="M3" s="56"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M4" s="57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M5" s="57"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="M6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -3726,120 +3733,120 @@
         <v>299</v>
       </c>
       <c r="K7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="M14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B15" t="s">
+        <v>367</v>
+      </c>
+      <c r="C15" t="s">
         <v>369</v>
       </c>
-      <c r="C15" t="s">
-        <v>371</v>
-      </c>
       <c r="D15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D18" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="M18" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -3847,24 +3854,24 @@
         <v>298</v>
       </c>
       <c r="C20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -3872,16 +3879,16 @@
         <v>298</v>
       </c>
       <c r="B22" t="s">
+        <v>362</v>
+      </c>
+      <c r="C22" t="s">
         <v>364</v>
       </c>
-      <c r="C22" t="s">
-        <v>366</v>
-      </c>
       <c r="D22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M22" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -3889,10 +3896,10 @@
         <v>298</v>
       </c>
       <c r="B23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -3900,16 +3907,16 @@
         <v>298</v>
       </c>
       <c r="B24" t="s">
+        <v>363</v>
+      </c>
+      <c r="C24" t="s">
         <v>365</v>
       </c>
-      <c r="C24" t="s">
-        <v>367</v>
-      </c>
       <c r="D24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M24" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -3919,73 +3926,73 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C26" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D27" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B28" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M29" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F30" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3995,10 +4002,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -4008,7 +4015,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -4016,7 +4023,7 @@
         <v>239</v>
       </c>
       <c r="D37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Twitch became silent again
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E9D14E-1903-43CD-80D7-C53185F1FCD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D2F6B3-073C-462B-A41E-AF51BCB886AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="2076" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="397">
   <si>
     <t>Guard</t>
   </si>
@@ -984,12 +984,6 @@
     <t>Haunt/Curse/Condemn</t>
   </si>
   <si>
-    <t>Haunt/Curse/ Condemn</t>
-  </si>
-  <si>
-    <t>Sleep/ Delusion</t>
-  </si>
-  <si>
     <t>Curse/Haunt/Weaken/ Delude/Sleep</t>
   </si>
   <si>
@@ -1231,13 +1225,16 @@
   </si>
   <si>
     <t>Morgan</t>
+  </si>
+  <si>
+    <t>Curse/ Condemn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1267,6 +1264,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1471,7 +1475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1541,6 +1545,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1860,7 +1867,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,23 +2279,23 @@
         <v>314</v>
       </c>
       <c r="B13" s="51" t="s">
+        <v>396</v>
+      </c>
+      <c r="C13" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="51" t="s">
         <v>315</v>
       </c>
-      <c r="C13" s="51" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>316</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>317</v>
-      </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="58" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="51"/>
       <c r="H13" s="51"/>
-      <c r="I13" s="51" t="s">
+      <c r="I13" s="58" t="s">
         <v>80</v>
       </c>
       <c r="J13" s="51" t="s">
@@ -2297,8 +2304,8 @@
       <c r="K13" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="L13" s="51" t="s">
-        <v>79</v>
+      <c r="L13" s="58" t="s">
+        <v>151</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>312</v>
@@ -2964,7 +2971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B53968-0167-4F4F-BD4B-0794225E238B}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3207,8 +3214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F22D4E-FC21-4D0F-B535-11FE6D9F512D}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView zoomScale="72" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3589,21 +3596,24 @@
       <c r="A28" s="2" t="s">
         <v>218</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>220</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3611,10 +3621,7 @@
         <v>221</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3663,62 +3670,62 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="M1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L2" s="55" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M2" s="56" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L3" s="55"/>
       <c r="M3" s="56"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M4" s="57" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="L5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M5" s="57"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="M6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -3726,120 +3733,120 @@
         <v>299</v>
       </c>
       <c r="K7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L8" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="J14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="M14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B15" t="s">
+        <v>367</v>
+      </c>
+      <c r="C15" t="s">
         <v>369</v>
       </c>
-      <c r="C15" t="s">
-        <v>371</v>
-      </c>
       <c r="D15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J15" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M15" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F16" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C17" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J17" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D18" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J18" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="M18" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D19" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -3847,24 +3854,24 @@
         <v>298</v>
       </c>
       <c r="C20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D20" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M21" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -3872,16 +3879,16 @@
         <v>298</v>
       </c>
       <c r="B22" t="s">
+        <v>362</v>
+      </c>
+      <c r="C22" t="s">
         <v>364</v>
       </c>
-      <c r="C22" t="s">
-        <v>366</v>
-      </c>
       <c r="D22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M22" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -3889,10 +3896,10 @@
         <v>298</v>
       </c>
       <c r="B23" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -3900,16 +3907,16 @@
         <v>298</v>
       </c>
       <c r="B24" t="s">
+        <v>363</v>
+      </c>
+      <c r="C24" t="s">
         <v>365</v>
       </c>
-      <c r="C24" t="s">
-        <v>367</v>
-      </c>
       <c r="D24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M24" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -3919,73 +3926,73 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B26" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C26" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D27" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M27" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B28" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M28" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M29" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B30" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F30" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B32" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -3995,10 +4002,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B34" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -4008,7 +4015,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -4016,7 +4023,7 @@
         <v>239</v>
       </c>
       <c r="D37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new Permissions, fix thingies
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D6B3C-E5FC-4AD8-A332-DB18FCFA42CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51952EE-B4B2-4868-8C75-C5CE68CF6272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="566">
   <si>
     <t>Guard</t>
   </si>
@@ -55,9 +57,6 @@
     <t>Aqua Squire</t>
   </si>
   <si>
-    <t>Ragnarök</t>
-  </si>
-  <si>
     <t>Quake</t>
   </si>
   <si>
@@ -961,33 +960,12 @@
     <t>Scrapper</t>
   </si>
   <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>multiplier</t>
-  </si>
-  <si>
-    <t>extra (Djinn, Equipment, ..)</t>
-  </si>
-  <si>
     <t>Bind</t>
   </si>
   <si>
     <t>Protect</t>
   </si>
   <si>
-    <t>Haunt/Curse/Condemn</t>
-  </si>
-  <si>
-    <t>Curse/Haunt/Weaken/ Delude/Sleep</t>
-  </si>
-  <si>
     <t>Notes for Tolbi:</t>
   </si>
   <si>
@@ -1742,13 +1720,31 @@
   </si>
   <si>
     <t>Soothing Star is not implemented.</t>
+  </si>
+  <si>
+    <t>Starburst</t>
+  </si>
+  <si>
+    <t>Ragnarok</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Poison/Taint</t>
+  </si>
+  <si>
+    <t>Unlock</t>
+  </si>
+  <si>
+    <t>Upgrade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1771,13 +1767,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2069,7 +2058,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2103,7 +2092,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2124,23 +2112,13 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -2152,6 +2130,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2470,7 +2463,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="A16" sqref="A16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2485,28 +2478,28 @@
     <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
     <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>305</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
@@ -2525,139 +2518,147 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>5</v>
+        <v>561</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>19</v>
-      </c>
       <c r="H2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>73</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>72</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="52" t="s">
-        <v>312</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>306</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>79</v>
+        <v>68</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="45" t="s">
-        <v>150</v>
+      <c r="D4" s="44" t="s">
+        <v>149</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="48" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>78</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>70</v>
+      <c r="A5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>69</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>151</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>150</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="42" t="s">
-        <v>80</v>
+        <v>24</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>79</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
@@ -2672,6 +2673,8 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -2686,235 +2689,247 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="C8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>32</v>
-      </c>
       <c r="K8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="C9" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="63" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="M9" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="N9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="40" t="s">
+      <c r="C11" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="L11" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="N11" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="K11" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="L11" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="46" t="s">
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
       <c r="I12" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="L12" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="M12" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
-        <v>314</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>396</v>
-      </c>
-      <c r="C13" s="58" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" s="58" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>315</v>
-      </c>
-      <c r="F13" s="58" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="J13" s="51" t="s">
-        <v>313</v>
-      </c>
-      <c r="K13" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="L13" s="58" t="s">
-        <v>151</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>312</v>
+      <c r="M12" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="53" t="s">
+        <v>560</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>388</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="53" t="s">
+        <v>562</v>
+      </c>
+      <c r="J13" s="53" t="s">
+        <v>307</v>
+      </c>
+      <c r="K13" s="53" t="s">
+        <v>563</v>
+      </c>
+      <c r="L13" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="M13" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="66" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -2930,6 +2945,8 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
@@ -2944,156 +2961,168 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>57</v>
-      </c>
       <c r="C16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>64</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>65</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>79</v>
+        <v>28</v>
+      </c>
+      <c r="F19" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
-        <v>85</v>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="46" t="s">
+        <v>84</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>82</v>
+      <c r="F20" s="29" t="s">
+        <v>81</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>26</v>
+      <c r="C21" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>7</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -3101,47 +3130,47 @@
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J24" t="s">
+        <v>117</v>
+      </c>
+      <c r="K24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
         <v>114</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J25" t="s">
         <v>118</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>115</v>
+      </c>
+      <c r="K26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>116</v>
+      </c>
+      <c r="K27" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I25" t="s">
-        <v>115</v>
-      </c>
-      <c r="J25" t="s">
-        <v>119</v>
-      </c>
-      <c r="K25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I26" t="s">
-        <v>116</v>
-      </c>
-      <c r="K26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="I27" t="s">
-        <v>117</v>
-      </c>
-      <c r="K27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="K29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3152,111 +3181,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0B7C81B-CCF0-4973-B9ED-154735BB83D5}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C1" t="s">
+        <v>565</v>
+      </c>
+      <c r="F1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G1" t="s">
+        <v>565</v>
+      </c>
+      <c r="J1" t="s">
+        <v>564</v>
+      </c>
+      <c r="K1" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" t="s">
         <v>30</v>
       </c>
-      <c r="B1">
-        <v>381</v>
-      </c>
-      <c r="C1">
-        <f>(B1-A1)/99</f>
-        <v>3.5454545454545454</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="B2">
-        <v>355</v>
-      </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C4" si="0">(B2-A2)/99</f>
-        <v>3.2525252525252526</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>32</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>-0.32323232323232326</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>-0.30303030303030304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5">
-        <f>AVERAGE(B1:B4)</f>
-        <v>368</v>
-      </c>
-      <c r="C5">
-        <f>AVERAGE(C1:C4)</f>
-        <v>1.5429292929292928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>303</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>304</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>307</v>
-      </c>
-      <c r="B9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C9" t="s">
-        <v>309</v>
-      </c>
-      <c r="D9" t="s">
-        <v>311</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>798</v>
-      </c>
-      <c r="C10">
-        <v>35</v>
-      </c>
-      <c r="D10">
-        <v>77</v>
-      </c>
-      <c r="E10">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <f>A10+(B10-A10)/99*C10</f>
-        <v>301.5151515151515</v>
-      </c>
-      <c r="D12">
-        <f>(B12+D10)*E10</f>
-        <v>719.17878787878783</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3269,7 +3332,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3282,155 +3345,155 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
         <v>123</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>125</v>
-      </c>
-      <c r="F1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3456,112 +3519,112 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
         <v>110</v>
-      </c>
-      <c r="C1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
         <v>95</v>
       </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4" t="s">
-        <v>96</v>
-      </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" t="s">
         <v>97</v>
       </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" t="s">
-        <v>98</v>
-      </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3589,230 +3652,230 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
         <v>152</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>153</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>154</v>
       </c>
-      <c r="E1" t="s">
-        <v>155</v>
-      </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J1" t="s">
         <v>183</v>
-      </c>
-      <c r="J1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
         <v>161</v>
       </c>
-      <c r="B2" t="s">
-        <v>162</v>
-      </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I2" t="s">
+        <v>184</v>
+      </c>
+      <c r="J2" t="s">
         <v>185</v>
-      </c>
-      <c r="J2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
         <v>166</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>167</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>168</v>
-      </c>
-      <c r="E7" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
-      </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="59"/>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="54"/>
+      <c r="B11" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="D11" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="E11" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="61" t="s">
-        <v>155</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="54"/>
+      <c r="C12" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60" t="s">
+      <c r="B13" s="57" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="D12" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>176</v>
-      </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="E13" s="64" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
+      <c r="C14" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="58"/>
+      <c r="E14" s="59" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="60" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="62" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="64" t="s">
+      <c r="B15" s="60" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="65" t="s">
-        <v>174</v>
-      </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3839,422 +3902,422 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -4279,360 +4342,360 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="L1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="M1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K2" t="s">
-        <v>344</v>
-      </c>
-      <c r="L2" s="55" t="s">
-        <v>357</v>
-      </c>
-      <c r="M2" s="56" t="s">
-        <v>354</v>
+        <v>336</v>
+      </c>
+      <c r="L2" s="67" t="s">
+        <v>349</v>
+      </c>
+      <c r="M2" s="68" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K3" t="s">
-        <v>344</v>
-      </c>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
+        <v>336</v>
+      </c>
+      <c r="L3" s="67"/>
+      <c r="M3" s="68"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="L4" t="s">
-        <v>351</v>
-      </c>
-      <c r="M4" s="57" t="s">
-        <v>355</v>
+        <v>343</v>
+      </c>
+      <c r="M4" s="69" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K5" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="L5" t="s">
-        <v>351</v>
-      </c>
-      <c r="M5" s="57"/>
+        <v>343</v>
+      </c>
+      <c r="M5" s="69"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K6" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="L6" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="M6" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K7" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="L7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="M7" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K8" t="s">
+        <v>344</v>
+      </c>
+      <c r="L8" t="s">
         <v>352</v>
       </c>
-      <c r="L8" t="s">
-        <v>360</v>
-      </c>
       <c r="M8" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="J14" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="M14" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="B15" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C15" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="D15" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="J15" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="M15" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D16" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F16" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="J16" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="M16" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="C17" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D17" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="J17" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="M17" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D18" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="J18" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="M18" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>321</v>
-      </c>
-      <c r="B19" s="54" t="s">
-        <v>370</v>
+        <v>313</v>
+      </c>
+      <c r="B19" s="52" t="s">
+        <v>362</v>
       </c>
       <c r="D19" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="J19" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="M19" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C20" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D20" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="M20" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="D21" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="M21" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="C22" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D22" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="M22" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B23" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="D23" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B24" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C24" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D24" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="M24" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B26" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="C26" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="M26" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B27" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="D27" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="M27" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B28" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="M28" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="M29" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B30" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="F30" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B32" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B34" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D37" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -4649,7 +4712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E22B74D-B8FD-400B-BAD2-C416C024FFE8}">
   <dimension ref="A1:A172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -4657,862 +4720,862 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change class requirements and unlocks
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEBD014-C9B3-4DE2-B820-13D96A8BD324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA51A74-F97D-4447-8DE0-B0D89CE74618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="601">
   <si>
     <t>Guard</t>
   </si>
@@ -1815,35 +1815,41 @@
     <t>Have Djinn</t>
   </si>
   <si>
-    <t>Visit Merc LH</t>
-  </si>
-  <si>
     <t>Unlock x Towns</t>
   </si>
   <si>
-    <t>Unlock x Dungeons</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
     <t>Default</t>
   </si>
   <si>
-    <t>Win 3 RPS</t>
-  </si>
-  <si>
     <t>Do an 8-ball?</t>
   </si>
   <si>
     <t>Unlocked Classes</t>
+  </si>
+  <si>
+    <t>Dungeons Completed</t>
+  </si>
+  <si>
+    <t>Win 4 RPS</t>
+  </si>
+  <si>
+    <t>Finish Merc LH</t>
+  </si>
+  <si>
+    <t>5 times in same town in a row or be on server for 30 days</t>
+  </si>
+  <si>
+    <t>Unlock x Dungeons or switch channels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1874,6 +1880,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2157,7 +2172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2275,6 +2290,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2594,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2612,6 +2630,7 @@
     <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.44140625" customWidth="1"/>
     <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -3347,34 +3366,34 @@
         <v>564</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="D38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="G38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="I38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K38" s="70" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L38" s="70"/>
       <c r="M38" s="70"/>
@@ -3385,34 +3404,34 @@
         <v>565</v>
       </c>
       <c r="B39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="G39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="H39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="K39" s="70" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L39" s="70"/>
       <c r="M39" s="70"/>
@@ -3490,69 +3509,83 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
       <c r="A43" s="70" t="s">
         <v>564</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="78" t="s">
         <v>585</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="78" t="s">
         <v>586</v>
       </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70" t="s">
+      <c r="D43" s="78" t="s">
+        <v>599</v>
+      </c>
+      <c r="E43" s="78" t="s">
         <v>587</v>
       </c>
-      <c r="F43" s="70" t="s">
+      <c r="F43" s="78" t="s">
         <v>588</v>
       </c>
-      <c r="G43" s="70" t="s">
+      <c r="G43" s="78" t="s">
         <v>589</v>
       </c>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70" t="s">
-        <v>592</v>
-      </c>
-      <c r="J43" s="70"/>
-      <c r="K43" s="70" t="s">
-        <v>596</v>
-      </c>
-      <c r="L43" s="70" t="s">
+      <c r="H43" s="81"/>
+      <c r="I43" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="M43" s="70" t="s">
+      <c r="J43" s="81"/>
+      <c r="K43" s="78" t="s">
         <v>597</v>
       </c>
-      <c r="N43" t="s">
-        <v>593</v>
+      <c r="L43" s="78" t="s">
+        <v>598</v>
+      </c>
+      <c r="M43" s="81" t="s">
+        <v>594</v>
+      </c>
+      <c r="N43" s="64" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="70" t="s">
         <v>565</v>
       </c>
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="78" t="s">
         <v>585</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70" t="s">
-        <v>598</v>
-      </c>
-      <c r="F44" s="70"/>
-      <c r="G44" s="70"/>
-      <c r="H44" s="70"/>
-      <c r="I44" s="70"/>
-      <c r="J44" s="70"/>
-      <c r="K44" s="70" t="s">
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="78" t="s">
+        <v>595</v>
+      </c>
+      <c r="F44" s="78" t="s">
+        <v>595</v>
+      </c>
+      <c r="G44" s="78" t="s">
+        <v>585</v>
+      </c>
+      <c r="H44" s="81"/>
+      <c r="I44" s="78" t="s">
+        <v>596</v>
+      </c>
+      <c r="J44" s="78" t="s">
+        <v>585</v>
+      </c>
+      <c r="K44" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="L44" s="70"/>
-      <c r="M44" s="70" t="s">
+      <c r="L44" s="78" t="s">
+        <v>596</v>
+      </c>
+      <c r="M44" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="N44" s="70"/>
+      <c r="N44" s="78" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="70"/>

</xml_diff>

<commit_message>
Fortune Teller and more
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA51A74-F97D-4447-8DE0-B0D89CE74618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17C9C2C-B144-4496-BB4D-BDB3FC97ACF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="603">
   <si>
     <t>Guard</t>
   </si>
@@ -1843,6 +1843,12 @@
   </si>
   <si>
     <t>Unlock x Dungeons or switch channels</t>
+  </si>
+  <si>
+    <t>Write in Colosso talks</t>
+  </si>
+  <si>
+    <t>Wear cursed gear</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1900,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1958,6 +1964,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2172,7 +2184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2293,6 +2305,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2612,8 +2630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2621,7 +2639,7 @@
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
@@ -3509,7 +3527,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="70" t="s">
         <v>564</v>
       </c>
@@ -3535,7 +3553,9 @@
       <c r="I43" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="J43" s="81"/>
+      <c r="J43" s="83" t="s">
+        <v>601</v>
+      </c>
       <c r="K43" s="78" t="s">
         <v>597</v>
       </c>
@@ -3556,8 +3576,12 @@
       <c r="B44" s="78" t="s">
         <v>585</v>
       </c>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
+      <c r="C44" s="78" t="s">
+        <v>602</v>
+      </c>
+      <c r="D44" s="82" t="s">
+        <v>133</v>
+      </c>
       <c r="E44" s="78" t="s">
         <v>595</v>
       </c>

</xml_diff>

<commit_message>
Auto start in guilds
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17C9C2C-B144-4496-BB4D-BDB3FC97ACF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A8CF49-5FBC-4A84-8A9F-25747901A0BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="606">
   <si>
     <t>Guard</t>
   </si>
@@ -1818,9 +1818,6 @@
     <t>Unlock x Towns</t>
   </si>
   <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -1845,10 +1842,22 @@
     <t>Unlock x Dungeons or switch channels</t>
   </si>
   <si>
-    <t>Write in Colosso talks</t>
-  </si>
-  <si>
-    <t>Wear cursed gear</t>
+    <t>Wear cursed gear on Mage Set</t>
+  </si>
+  <si>
+    <t>Days active</t>
+  </si>
+  <si>
+    <t>Write in Colosso talks, Win a PvP battle</t>
+  </si>
+  <si>
+    <t>VenusDjinn</t>
+  </si>
+  <si>
+    <t>MarsDjinn</t>
+  </si>
+  <si>
+    <t>MercuryDjinn</t>
   </si>
 </sst>
 </file>
@@ -2307,10 +2316,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2631,7 +2640,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2643,9 +2652,9 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
     <col min="11" max="11" width="12.44140625" customWidth="1"/>
     <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.21875" bestFit="1" customWidth="1"/>
@@ -3384,72 +3393,72 @@
         <v>564</v>
       </c>
       <c r="B38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="H38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="J38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="K38" s="70" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L38" s="70"/>
       <c r="M38" s="70"/>
       <c r="N38" s="70"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="70" t="s">
         <v>565</v>
       </c>
       <c r="B39" s="70" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="C39" s="70" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="E39" s="70" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="F39" s="70" t="s">
-        <v>592</v>
+        <v>604</v>
       </c>
       <c r="G39" s="70" t="s">
-        <v>592</v>
+        <v>196</v>
       </c>
       <c r="H39" s="70" t="s">
-        <v>592</v>
+        <v>196</v>
       </c>
       <c r="I39" s="70" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
       <c r="J39" s="70" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
       <c r="K39" s="70" t="s">
-        <v>592</v>
+        <v>605</v>
       </c>
       <c r="L39" s="70"/>
       <c r="M39" s="70"/>
@@ -3527,7 +3536,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="70" t="s">
         <v>564</v>
       </c>
@@ -3538,7 +3547,7 @@
         <v>586</v>
       </c>
       <c r="D43" s="78" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E43" s="78" t="s">
         <v>587</v>
@@ -3553,23 +3562,23 @@
       <c r="I43" s="78" t="s">
         <v>591</v>
       </c>
-      <c r="J43" s="83" t="s">
-        <v>601</v>
+      <c r="J43" s="82" t="s">
+        <v>602</v>
       </c>
       <c r="K43" s="78" t="s">
+        <v>596</v>
+      </c>
+      <c r="L43" s="78" t="s">
         <v>597</v>
       </c>
-      <c r="L43" s="78" t="s">
-        <v>598</v>
-      </c>
-      <c r="M43" s="81" t="s">
-        <v>594</v>
+      <c r="M43" s="78" t="s">
+        <v>593</v>
       </c>
       <c r="N43" s="64" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="70" t="s">
         <v>565</v>
       </c>
@@ -3577,23 +3586,23 @@
         <v>585</v>
       </c>
       <c r="C44" s="78" t="s">
-        <v>602</v>
-      </c>
-      <c r="D44" s="82" t="s">
-        <v>133</v>
+        <v>600</v>
+      </c>
+      <c r="D44" s="83" t="s">
+        <v>601</v>
       </c>
       <c r="E44" s="78" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F44" s="78" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G44" s="78" t="s">
         <v>585</v>
       </c>
       <c r="H44" s="81"/>
       <c r="I44" s="78" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J44" s="78" t="s">
         <v>585</v>
@@ -3602,13 +3611,13 @@
         <v>590</v>
       </c>
       <c r="L44" s="78" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="M44" s="78" t="s">
         <v>590</v>
       </c>
       <c r="N44" s="78" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
do djinn work now....
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE8AF56-C1C5-42DF-B729-A711170EB61C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB8683A-0F28-48C6-A6F1-BE186C6DE8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="7" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="506">
   <si>
     <t>Guard</t>
   </si>
@@ -1215,36 +1215,12 @@
     <t>Stun Muscle is not implemented.</t>
   </si>
   <si>
-    <t>Human Hunt is not implemented.</t>
-  </si>
-  <si>
-    <t>Rumble is not implemented.</t>
-  </si>
-  <si>
     <t>Sonic Wave is not implemented.</t>
   </si>
   <si>
-    <t>Raging Flood is not implemented.</t>
-  </si>
-  <si>
-    <t>Rising Venom is not implemented.</t>
-  </si>
-  <si>
-    <t>Slaver is not implemented.</t>
-  </si>
-  <si>
     <t>Mesmerize is not implemented.</t>
   </si>
   <si>
-    <t>Electric Bite is not implemented.</t>
-  </si>
-  <si>
-    <t>Fortify is not implemented.</t>
-  </si>
-  <si>
-    <t>Poison Sting is not implemented.</t>
-  </si>
-  <si>
     <t>Punish is not implemented.</t>
   </si>
   <si>
@@ -1257,9 +1233,6 @@
     <t>Double Chop is not implemented.</t>
   </si>
   <si>
-    <t>Poison Ink is not implemented.</t>
-  </si>
-  <si>
     <t>Scornful Caress is not implemented.</t>
   </si>
   <si>
@@ -1275,21 +1248,12 @@
     <t>Fire Blessing is not implemented.</t>
   </si>
   <si>
-    <t>Recovery is not implemented.</t>
-  </si>
-  <si>
-    <t>Mucous Gel is not implemented.</t>
-  </si>
-  <si>
     <t>Bloodcurdle is not implemented.</t>
   </si>
   <si>
     <t>Cold Snap is not implemented.</t>
   </si>
   <si>
-    <t>Mystic Flame is not implemented.</t>
-  </si>
-  <si>
     <t>Out of Order is not implemented.</t>
   </si>
   <si>
@@ -1302,93 +1266,45 @@
     <t>Djinn Burp is not implemented.</t>
   </si>
   <si>
-    <t>Power Bite is not implemented.</t>
-  </si>
-  <si>
     <t>Terrible Bite is not implemented.</t>
   </si>
   <si>
-    <t>Flying Attack is not implemented.</t>
-  </si>
-  <si>
     <t>Swift Strike is not implemented.</t>
   </si>
   <si>
-    <t>Freebite Rush is not implemented.</t>
-  </si>
-  <si>
     <t>Djinn Blast is not implemented.</t>
   </si>
   <si>
-    <t>Earth Force is not implemented.</t>
-  </si>
-  <si>
     <t>Cruel Ruin is not implemented.</t>
   </si>
   <si>
     <t>Djinn Storm is not implemented.</t>
   </si>
   <si>
-    <t>Numbing Sting is not implemented.</t>
-  </si>
-  <si>
     <t>Charon is not implemented.</t>
   </si>
   <si>
     <t>Element Swap is not implemented.</t>
   </si>
   <si>
-    <t>Formina Sage is not implemented.</t>
-  </si>
-  <si>
     <t>Crucible is not implemented.</t>
   </si>
   <si>
     <t>Dark Contact is not implemented.</t>
   </si>
   <si>
-    <t>Mortal Blow is not implemented.</t>
-  </si>
-  <si>
-    <t>Regen Dance is not implemented.</t>
-  </si>
-  <si>
-    <t>Flame Breath is not implemented.</t>
-  </si>
-  <si>
     <t>Djinnfest is not implemented.</t>
   </si>
   <si>
-    <t>Heat Kiss is not implemented.</t>
-  </si>
-  <si>
-    <t>Flash Punch is not implemented.</t>
-  </si>
-  <si>
     <t>Drag Down is not implemented.</t>
   </si>
   <si>
     <t>Seething Rage is not implemented.</t>
   </si>
   <si>
-    <t>Outer Space is not implemented.</t>
-  </si>
-  <si>
-    <t>Evil Blessing is not implemented.</t>
-  </si>
-  <si>
-    <t>Severe Blow is not implemented.</t>
-  </si>
-  <si>
     <t>Consume Djinn is not implemented.</t>
   </si>
   <si>
-    <t>Hydro Slash is not implemented.</t>
-  </si>
-  <si>
-    <t>Forcible Arm is not implemented.</t>
-  </si>
-  <si>
     <t>Crazy Voice is not implemented.</t>
   </si>
   <si>
@@ -1404,12 +1320,6 @@
     <t>Frostbite is not implemented.</t>
   </si>
   <si>
-    <t>Spinning Beat is not implemented.</t>
-  </si>
-  <si>
-    <t>Poison Beat is not implemented.</t>
-  </si>
-  <si>
     <t>Cyclone Slash is not implemented.</t>
   </si>
   <si>
@@ -1428,33 +1338,15 @@
     <t>Pure Hatred is not implemented.</t>
   </si>
   <si>
-    <t>Mad Spatter is not implemented.</t>
-  </si>
-  <si>
-    <t>Maneater is not implemented.</t>
-  </si>
-  <si>
-    <t>Onslaught is not implemented.</t>
-  </si>
-  <si>
     <t>Electric Sting is not implemented.</t>
   </si>
   <si>
-    <t>Lucid Prophecy is not implemented.</t>
-  </si>
-  <si>
     <t>Fiery Juggle is not implemented.</t>
   </si>
   <si>
-    <t>Sack is not implemented.</t>
-  </si>
-  <si>
     <t>Seethe is not implemented.</t>
   </si>
   <si>
-    <t>Quick Slash is not implemented.</t>
-  </si>
-  <si>
     <t>Nerve Shattering Shriek is not implemented.</t>
   </si>
   <si>
@@ -1467,36 +1359,15 @@
     <t>Upward Blast is not implemented.</t>
   </si>
   <si>
-    <t>Sticky Goo is not implemented.</t>
-  </si>
-  <si>
     <t>Speed Surge is not implemented.</t>
   </si>
   <si>
     <t>Divide is not implemented.</t>
   </si>
   <si>
-    <t>Spasm is not implemented.</t>
-  </si>
-  <si>
-    <t>Stand Ready is not implemented.</t>
-  </si>
-  <si>
-    <t>Ocean Fist is not implemented.</t>
-  </si>
-  <si>
-    <t>Typhoon Blow is not implemented.</t>
-  </si>
-  <si>
-    <t>Watery Grave is not implemented.</t>
-  </si>
-  <si>
     <t>Speed Slice is not implemented.</t>
   </si>
   <si>
-    <t>Spider Web is not implemented.</t>
-  </si>
-  <si>
     <t>Arid Blast is not implemented.</t>
   </si>
   <si>
@@ -1509,9 +1380,6 @@
     <t>Poison Flow is not implemented.</t>
   </si>
   <si>
-    <t>Kill Sting is not implemented.</t>
-  </si>
-  <si>
     <t>Call Skull is not implemented.</t>
   </si>
   <si>
@@ -1524,9 +1392,6 @@
     <t>Healing is not implemented.</t>
   </si>
   <si>
-    <t>Poison Gel is not implemented.</t>
-  </si>
-  <si>
     <t>Stifle Shot is not implemented.</t>
   </si>
   <si>
@@ -1545,9 +1410,6 @@
     <t>Examine Situation is not implemented.</t>
   </si>
   <si>
-    <t>Storm Blessing is not implemented.</t>
-  </si>
-  <si>
     <t>Paralysis Shot is not implemented.</t>
   </si>
   <si>
@@ -1557,9 +1419,6 @@
     <t>Stun Jip is not implemented.</t>
   </si>
   <si>
-    <t>Soothing Star is not implemented.</t>
-  </si>
-  <si>
     <t>Starburst</t>
   </si>
   <si>
@@ -1699,28 +1558,13 @@
   </si>
   <si>
     <t>Star Burst is not implemented.</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>not important yet</t>
-  </si>
-  <si>
-    <t>nope</t>
-  </si>
-  <si>
-    <t>damages PP</t>
-  </si>
-  <si>
-    <t>later</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1758,14 +1602,6 @@
     <font>
       <b/>
       <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2057,7 +1893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2186,7 +2022,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2561,7 +2396,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>507</v>
+        <v>460</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>71</v>
@@ -2937,7 +2772,7 @@
     </row>
     <row r="13" spans="1:14" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="53" t="s">
-        <v>506</v>
+        <v>459</v>
       </c>
       <c r="B13" s="49" t="s">
         <v>388</v>
@@ -2957,13 +2792,13 @@
       <c r="G13" s="49"/>
       <c r="H13" s="49"/>
       <c r="I13" s="53" t="s">
-        <v>508</v>
+        <v>461</v>
       </c>
       <c r="J13" s="53" t="s">
         <v>307</v>
       </c>
       <c r="K13" s="53" t="s">
-        <v>509</v>
+        <v>462</v>
       </c>
       <c r="L13" s="53" t="s">
         <v>150</v>
@@ -3255,37 +3090,37 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="67" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="B38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="C38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="D38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="E38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="F38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="G38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="H38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="I38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="J38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="K38" s="67" t="s">
-        <v>538</v>
+        <v>491</v>
       </c>
       <c r="L38" s="67"/>
       <c r="M38" s="67"/>
@@ -3293,22 +3128,22 @@
     </row>
     <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="67" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="B39" s="67" t="s">
-        <v>549</v>
+        <v>502</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>549</v>
+        <v>502</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>550</v>
+        <v>503</v>
       </c>
       <c r="E39" s="67" t="s">
-        <v>550</v>
+        <v>503</v>
       </c>
       <c r="F39" s="67" t="s">
-        <v>550</v>
+        <v>503</v>
       </c>
       <c r="G39" s="67" t="s">
         <v>196</v>
@@ -3317,13 +3152,13 @@
         <v>196</v>
       </c>
       <c r="I39" s="67" t="s">
-        <v>551</v>
+        <v>504</v>
       </c>
       <c r="J39" s="67" t="s">
-        <v>551</v>
+        <v>504</v>
       </c>
       <c r="K39" s="67" t="s">
-        <v>551</v>
+        <v>504</v>
       </c>
       <c r="L39" s="67"/>
       <c r="M39" s="67"/>
@@ -3403,86 +3238,86 @@
     </row>
     <row r="43" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="67" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="B43" s="75" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
       <c r="C43" s="75" t="s">
-        <v>532</v>
+        <v>485</v>
       </c>
       <c r="D43" s="75" t="s">
-        <v>544</v>
+        <v>497</v>
       </c>
       <c r="E43" s="75" t="s">
-        <v>533</v>
+        <v>486</v>
       </c>
       <c r="F43" s="75" t="s">
-        <v>534</v>
+        <v>487</v>
       </c>
       <c r="G43" s="75" t="s">
-        <v>535</v>
+        <v>488</v>
       </c>
       <c r="H43" s="78"/>
       <c r="I43" s="75" t="s">
-        <v>537</v>
+        <v>490</v>
       </c>
       <c r="J43" s="79" t="s">
-        <v>548</v>
+        <v>501</v>
       </c>
       <c r="K43" s="75" t="s">
-        <v>542</v>
+        <v>495</v>
       </c>
       <c r="L43" s="75" t="s">
-        <v>543</v>
+        <v>496</v>
       </c>
       <c r="M43" s="75" t="s">
-        <v>539</v>
+        <v>492</v>
       </c>
       <c r="N43" s="64" t="s">
-        <v>545</v>
+        <v>498</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="67" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="B44" s="75" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
       <c r="C44" s="75" t="s">
-        <v>546</v>
+        <v>499</v>
       </c>
       <c r="D44" s="80" t="s">
-        <v>547</v>
+        <v>500</v>
       </c>
       <c r="E44" s="75" t="s">
-        <v>540</v>
+        <v>493</v>
       </c>
       <c r="F44" s="75" t="s">
-        <v>540</v>
+        <v>493</v>
       </c>
       <c r="G44" s="75" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
       <c r="H44" s="78"/>
       <c r="I44" s="75" t="s">
-        <v>541</v>
+        <v>494</v>
       </c>
       <c r="J44" s="75" t="s">
-        <v>531</v>
+        <v>484</v>
       </c>
       <c r="K44" s="75" t="s">
-        <v>536</v>
+        <v>489</v>
       </c>
       <c r="L44" s="75" t="s">
-        <v>541</v>
+        <v>494</v>
       </c>
       <c r="M44" s="75" t="s">
-        <v>536</v>
+        <v>489</v>
       </c>
       <c r="N44" s="75" t="s">
-        <v>541</v>
+        <v>494</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -3547,7 +3382,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="67" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="B48" s="67"/>
       <c r="C48" s="67"/>
@@ -3565,7 +3400,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="67" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="B49" s="67"/>
       <c r="C49" s="67"/>
@@ -3654,25 +3489,25 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="C1" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="F1" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="G1" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="J1" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="K1" t="s">
-        <v>511</v>
+        <v>464</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>515</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -3683,16 +3518,16 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>525</v>
+        <v>478</v>
       </c>
       <c r="G2" t="s">
-        <v>526</v>
+        <v>479</v>
       </c>
       <c r="I2" t="s">
         <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>512</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -3703,16 +3538,16 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>527</v>
+        <v>480</v>
       </c>
       <c r="G3" t="s">
-        <v>528</v>
+        <v>481</v>
       </c>
       <c r="I3" t="s">
         <v>56</v>
       </c>
       <c r="N3" t="s">
-        <v>513</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -3726,7 +3561,7 @@
         <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>514</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3740,7 +3575,7 @@
         <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>516</v>
+        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3754,7 +3589,7 @@
         <v>59</v>
       </c>
       <c r="N6" t="s">
-        <v>517</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -3765,13 +3600,13 @@
         <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>529</v>
+        <v>482</v>
       </c>
       <c r="I7" t="s">
         <v>60</v>
       </c>
       <c r="N7" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3782,7 +3617,7 @@
         <v>47</v>
       </c>
       <c r="N8" t="s">
-        <v>519</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -3793,7 +3628,7 @@
         <v>52</v>
       </c>
       <c r="N9" t="s">
-        <v>520</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -3804,7 +3639,7 @@
         <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>530</v>
+        <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -3838,7 +3673,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>521</v>
+        <v>474</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -3849,7 +3684,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>524</v>
+        <v>477</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -3860,7 +3695,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>522</v>
+        <v>475</v>
       </c>
       <c r="B21">
         <v>30</v>
@@ -3871,7 +3706,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>523</v>
+        <v>476</v>
       </c>
       <c r="B22">
         <v>40</v>
@@ -5269,686 +5104,374 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E22B74D-B8FD-400B-BAD2-C416C024FFE8}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:A71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="84"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>485</v>
-      </c>
-      <c r="E2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>413</v>
       </c>
-      <c r="E3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="84"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>490</v>
-      </c>
-      <c r="E5" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>407</v>
       </c>
-      <c r="E6" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>430</v>
       </c>
-      <c r="E7" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>414</v>
-      </c>
-      <c r="E8" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>446</v>
-      </c>
-      <c r="E9" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>449</v>
       </c>
-      <c r="E12" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>433</v>
-      </c>
-      <c r="E13" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>427</v>
       </c>
-      <c r="E14" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>492</v>
-      </c>
-      <c r="E15" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>456</v>
       </c>
-      <c r="E16" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>409</v>
-      </c>
-      <c r="E17" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>434</v>
-      </c>
-      <c r="E18" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>408</v>
-      </c>
-      <c r="E19" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>477</v>
-      </c>
-      <c r="E23" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>425</v>
-      </c>
-      <c r="E24" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>419</v>
-      </c>
-      <c r="E25" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>428</v>
-      </c>
-      <c r="E26" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>503</v>
-      </c>
-      <c r="E27" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>438</v>
-      </c>
-      <c r="E28" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>404</v>
-      </c>
-      <c r="E29" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>441</v>
-      </c>
-      <c r="E31" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>459</v>
-      </c>
-      <c r="E33" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>432</v>
+        <v>397</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>399</v>
+        <v>451</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>493</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>439</v>
+        <v>453</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>391</v>
+        <v>444</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>447</v>
+        <v>391</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>457</v>
+        <v>505</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>489</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>466</v>
+        <v>437</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>463</v>
+        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>397</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>415</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>471</v>
+        <v>408</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A128">
-    <sortCondition ref="A128"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A127">
+    <sortCondition ref="A127"/>
   </sortState>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Iron out a couple of christmas bugs
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet (version 1).xlsx
+++ b/IodemBot/IodemClassSheet (version 1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9EFAA4-827B-4339-9BD9-C3B77BCBA4C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983F5A19-F577-4157-AD13-9B5CB4DDA151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="568">
   <si>
     <t>Guard</t>
   </si>
@@ -1676,13 +1676,82 @@
   </si>
   <si>
     <t>Virtuous Armlet</t>
+  </si>
+  <si>
+    <t>Dracoholt</t>
+  </si>
+  <si>
+    <t>Acrobat</t>
+  </si>
+  <si>
+    <t>Reaper</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Joker</t>
+  </si>
+  <si>
+    <t>Ace</t>
+  </si>
+  <si>
+    <t>(idk if 4)</t>
+  </si>
+  <si>
+    <t>Harlequin</t>
+  </si>
+  <si>
+    <t>Beast Lord</t>
+  </si>
+  <si>
+    <t>Beast Keeper</t>
+  </si>
+  <si>
+    <t>Crypt Lord</t>
+  </si>
+  <si>
+    <t>Necromage</t>
+  </si>
+  <si>
+    <t>Apostate</t>
+  </si>
+  <si>
+    <t>Dracobolt</t>
+  </si>
+  <si>
+    <t>Baffle Card</t>
+  </si>
+  <si>
+    <t>Sword Card</t>
+  </si>
+  <si>
+    <t>Flame Card</t>
+  </si>
+  <si>
+    <t>Sleep Card</t>
+  </si>
+  <si>
+    <t>Thunder Card</t>
+  </si>
+  <si>
+    <t>Death Card</t>
+  </si>
+  <si>
+    <t>Bramble Card</t>
+  </si>
+  <si>
+    <t>Frost Card</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1719,6 +1788,14 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2023,7 +2100,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2144,6 +2221,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2152,15 +2235,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{96F5CFF9-578C-433E-B401-E4A3F8FFBEAD}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2528,7 +2625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I24" sqref="I24:K29"/>
     </sheetView>
   </sheetViews>
@@ -3272,7 +3369,7 @@
       <c r="M38" s="67"/>
       <c r="N38" s="67"/>
     </row>
-    <row r="39" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="67" t="s">
         <v>441</v>
       </c>
@@ -3342,7 +3439,7 @@
       <c r="M41" s="67"/>
       <c r="N41" s="67"/>
     </row>
-    <row r="42" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="67"/>
       <c r="B42" s="71" t="s">
         <v>28</v>
@@ -3870,10 +3967,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3034823A-014A-402D-994F-F4A05E7ABD19}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3882,6 +3979,9 @@
     <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
@@ -3933,14 +4033,14 @@
       <c r="G3" t="s">
         <v>492</v>
       </c>
-      <c r="I3" s="81" t="s">
+      <c r="I3" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81" t="s">
+      <c r="J3" s="85"/>
+      <c r="K3" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="81"/>
+      <c r="L3" s="85"/>
       <c r="M3" t="s">
         <v>98</v>
       </c>
@@ -4106,6 +4206,9 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>545</v>
+      </c>
       <c r="E12" t="s">
         <v>115</v>
       </c>
@@ -4257,6 +4360,218 @@
     <row r="29" spans="5:10" x14ac:dyDescent="0.3">
       <c r="J29" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C34" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>546</v>
+      </c>
+      <c r="E34" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" s="88" t="s">
+        <v>513</v>
+      </c>
+      <c r="G34" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="H34" s="88" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C35" s="89" t="s">
+        <v>548</v>
+      </c>
+      <c r="D35" s="89" t="s">
+        <v>549</v>
+      </c>
+      <c r="E35" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="89" t="s">
+        <v>548</v>
+      </c>
+      <c r="H35" s="89" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="81" t="s">
+        <v>546</v>
+      </c>
+      <c r="E36" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="81" t="s">
+        <v>513</v>
+      </c>
+      <c r="G36" s="81" t="s">
+        <v>98</v>
+      </c>
+      <c r="H36" s="81" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C37" s="81" t="s">
+        <v>550</v>
+      </c>
+      <c r="D37" s="81" t="s">
+        <v>553</v>
+      </c>
+      <c r="E37" s="81" t="s">
+        <v>555</v>
+      </c>
+      <c r="F37" s="81" t="s">
+        <v>514</v>
+      </c>
+      <c r="G37" s="81" t="s">
+        <v>556</v>
+      </c>
+      <c r="H37" s="81" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="81" t="s">
+        <v>551</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="81" t="s">
+        <v>554</v>
+      </c>
+      <c r="F38" s="81" t="s">
+        <v>515</v>
+      </c>
+      <c r="G38" s="81" t="s">
+        <v>557</v>
+      </c>
+      <c r="H38" s="81" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C40" s="81" t="s">
+        <v>560</v>
+      </c>
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="81" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="81" t="s">
+        <v>508</v>
+      </c>
+      <c r="H40" s="81" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="81" t="s">
+        <v>561</v>
+      </c>
+      <c r="D41" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" t="s">
+        <v>489</v>
+      </c>
+      <c r="F41" s="81" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="81" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="81" t="s">
+        <v>562</v>
+      </c>
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" t="s">
+        <v>492</v>
+      </c>
+      <c r="F42" s="81" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C43" s="81" t="s">
+        <v>563</v>
+      </c>
+      <c r="E43" t="s">
+        <v>500</v>
+      </c>
+      <c r="F43" s="81" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C44" s="81" t="s">
+        <v>564</v>
+      </c>
+      <c r="E44" t="s">
+        <v>503</v>
+      </c>
+      <c r="F44" s="81" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="81" t="s">
+        <v>565</v>
+      </c>
+      <c r="E45" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C46" s="81" t="s">
+        <v>566</v>
+      </c>
+      <c r="E46" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="81" t="s">
+        <v>567</v>
+      </c>
+      <c r="E47" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E48" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="81" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -4264,7 +4579,11 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
+  <conditionalFormatting sqref="F43:F44">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4400,7 +4719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21AE0FE-0550-4A50-A428-F4972BDBD2F3}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -4424,17 +4743,17 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="82" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="82" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="83" t="s">
         <v>529</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -4470,7 +4789,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="83" t="s">
         <v>530</v>
       </c>
       <c r="E5" t="s">
@@ -4591,7 +4910,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="84" t="s">
         <v>535</v>
       </c>
       <c r="G10" t="s">
@@ -5323,7 +5642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FC84A19-D4A7-4A92-BABE-05F233968AC8}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
@@ -5348,10 +5667,10 @@
       <c r="K2" t="s">
         <v>313</v>
       </c>
-      <c r="L2" s="82" t="s">
+      <c r="L2" s="86" t="s">
         <v>326</v>
       </c>
-      <c r="M2" s="83" t="s">
+      <c r="M2" s="87" t="s">
         <v>323</v>
       </c>
     </row>
@@ -5359,8 +5678,8 @@
       <c r="K3" t="s">
         <v>313</v>
       </c>
-      <c r="L3" s="82"/>
-      <c r="M3" s="83"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K4" t="s">
@@ -5369,7 +5688,7 @@
       <c r="L4" t="s">
         <v>320</v>
       </c>
-      <c r="M4" s="81" t="s">
+      <c r="M4" s="85" t="s">
         <v>324</v>
       </c>
     </row>
@@ -5380,7 +5699,7 @@
       <c r="L5" t="s">
         <v>320</v>
       </c>
-      <c r="M5" s="81"/>
+      <c r="M5" s="85"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="K6" t="s">

</xml_diff>